<commit_message>
:bug: fix: solve timeout problem not available on windows
</commit_message>
<xml_diff>
--- a/data/processed/AMOSTRA_e-SIC_processed.xlsx
+++ b/data/processed/AMOSTRA_e-SIC_processed.xlsx
@@ -655,13 +655,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -768,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -952,10 +952,10 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -964,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
@@ -1295,7 +1295,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1684,13 +1684,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1699,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1834,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -1846,7 +1846,7 @@
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" t="n">
         <v>1</v>
@@ -1929,7 +1929,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -1978,13 +1978,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1993,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -2027,13 +2027,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -2042,7 +2042,7 @@
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -2076,13 +2076,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -2091,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -2140,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" t="n">
         <v>1</v>
@@ -2275,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -2321,7 +2321,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -2336,7 +2336,7 @@
         <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
@@ -2370,13 +2370,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -2385,7 +2385,7 @@
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -2419,13 +2419,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -2912,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -2924,7 +2924,7 @@
         <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
@@ -3120,7 +3120,7 @@
         <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
@@ -3154,13 +3154,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -3169,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
@@ -3252,7 +3252,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" t="n">
         <v>0</v>
@@ -3267,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="H58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
@@ -3353,7 +3353,7 @@
         <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -3405,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>1</v>
@@ -3414,7 +3414,7 @@
         <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>
@@ -3451,7 +3451,7 @@
         <v>1</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -3693,7 +3693,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
@@ -3708,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="H67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" t="n">
         <v>0</v>
@@ -3742,13 +3742,13 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
@@ -3757,7 +3757,7 @@
         <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" t="n">
         <v>0</v>
@@ -3846,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
@@ -3855,7 +3855,7 @@
         <v>0</v>
       </c>
       <c r="H70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" t="n">
         <v>1</v>
@@ -3938,13 +3938,13 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72" t="n">
         <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>0</v>
@@ -3953,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="H72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" t="n">
         <v>0</v>
@@ -3987,13 +3987,13 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73" t="n">
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -4002,7 +4002,7 @@
         <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73" t="n">
         <v>0</v>
@@ -4039,10 +4039,10 @@
         <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
@@ -4051,7 +4051,7 @@
         <v>0</v>
       </c>
       <c r="H74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" t="n">
         <v>1</v>
@@ -4189,7 +4189,7 @@
         <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
@@ -4198,7 +4198,7 @@
         <v>0</v>
       </c>
       <c r="H77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I77" t="n">
         <v>1</v>
@@ -4627,7 +4627,7 @@
         <v>1</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
@@ -4639,7 +4639,7 @@
         <v>1</v>
       </c>
       <c r="H86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86" t="n">
         <v>1</v>
@@ -4673,13 +4673,13 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -4688,7 +4688,7 @@
         <v>0</v>
       </c>
       <c r="H87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I87" t="n">
         <v>0</v>
@@ -4771,13 +4771,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>0</v>
@@ -4786,7 +4786,7 @@
         <v>0</v>
       </c>
       <c r="H89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" t="n">
         <v>0</v>
@@ -5016,7 +5016,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
@@ -5031,7 +5031,7 @@
         <v>0</v>
       </c>
       <c r="H94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I94" t="n">
         <v>0</v>
@@ -5120,7 +5120,7 @@
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>1</v>
@@ -5129,7 +5129,7 @@
         <v>0</v>
       </c>
       <c r="H96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96" t="n">
         <v>0</v>
@@ -5215,7 +5215,7 @@
         <v>1</v>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
@@ -5261,13 +5261,13 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D99" t="n">
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
@@ -5276,7 +5276,7 @@
         <v>0</v>
       </c>
       <c r="H99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99" t="n">
         <v>0</v>
@@ -5313,7 +5313,7 @@
         <v>1</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" t="n">
         <v>1</v>
@@ -5325,7 +5325,7 @@
         <v>1</v>
       </c>
       <c r="H100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I100" t="n">
         <v>1</v>

</xml_diff>